<commit_message>
Doleance_edit - modif date debut - modif date fin
</commit_message>
<xml_diff>
--- a/static/files/devis.xlsx
+++ b/static/files/devis.xlsx
@@ -1580,7 +1580,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="H10:H43"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B38:C38"/>
@@ -1592,6 +1591,7 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B15:C15"/>
@@ -1603,7 +1603,7 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="I11:I12"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.59055118110236" right="0.13" top="0.35433070866142" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup orientation="portrait" paperSize="9" scale="76" fitToHeight="0"/>

</xml_diff>

<commit_message>
Liste interventions sur la page doleances
</commit_message>
<xml_diff>
--- a/static/files/devis.xlsx
+++ b/static/files/devis.xlsx
@@ -850,7 +850,7 @@
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>0035/GDP/24H</t>
+          <t>2195/SMPVE/24C</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="J3" s="40" t="inlineStr">
         <is>
-          <t>Hors Contrat</t>
+          <t>Conso</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="C6" s="13" t="inlineStr">
         <is>
-          <t>GDP / AINA</t>
+          <t>SMPVE / DMSA</t>
         </is>
       </c>
     </row>
@@ -908,7 +908,7 @@
       </c>
       <c r="C7" s="41" t="inlineStr">
         <is>
-          <t>PANNE</t>
+          <t>RECUPERATIONS ET EXPEDITIONS DES BIDONS DE 20L.</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>07/11/2024 12:26</t>
+          <t>11/12/2024 08:00</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
@@ -1591,19 +1591,19 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B11:C12"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="I11:I12"/>
-    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.59055118110236" right="0.13" top="0.35433070866142" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup orientation="portrait" paperSize="9" scale="76" fitToHeight="0"/>

</xml_diff>